<commit_message>
Just starting to break code into main/suppl. files.
I realized that there will be a decent amount of analysis that is not
relevant to the final results of the manuscript, and that anyone looking
to reproduce the analyses may be annoyed at having to differentiate
between the 'real' code and the supporting code. So this commit is just
after I started working on an Rmarkdown document for the supporting
code, but before breaking out the dataprep and main analysis .R files.
</commit_message>
<xml_diff>
--- a/data/field_ecology_data.xlsx
+++ b/data/field_ecology_data.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="27760" windowHeight="14220" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="27760" windowHeight="14220"/>
   </bookViews>
   <sheets>
-    <sheet name="raw data" sheetId="1" r:id="rId1"/>
-    <sheet name="soil moisture" sheetId="2" r:id="rId2"/>
-    <sheet name="LSRecolanalyze" sheetId="6" r:id="rId3"/>
-    <sheet name="LSRecolminuszeros" sheetId="3" r:id="rId4"/>
-    <sheet name="Ecol paired" sheetId="4" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId1"/>
+    <sheet name="raw data" sheetId="1" r:id="rId2"/>
+    <sheet name="soil moisture" sheetId="2" r:id="rId3"/>
+    <sheet name="LSRecolanalyze" sheetId="6" r:id="rId4"/>
+    <sheet name="LSRecolminuszeros" sheetId="3" r:id="rId5"/>
+    <sheet name="Ecol paired" sheetId="4" r:id="rId6"/>
     <sheet name="LSRecol1" sheetId="5" r:id="rId7"/>
   </sheets>
   <externalReferences>
@@ -305,9 +305,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.0000"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -489,26 +489,26 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -532,6 +532,7 @@
       <sheetName val="Reg"/>
       <sheetName val="RegArray"/>
       <sheetName val="Temp"/>
+      <sheetName val="PopTools.xla"/>
     </sheetNames>
     <definedNames>
       <definedName name="ResampleRows"/>
@@ -542,6 +543,7 @@
       <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
       <sheetData sheetId="4"/>
+      <sheetData sheetId="5" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -869,11 +871,2350 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet7" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:M52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="8.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5" style="15" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.83203125" style="15" customWidth="1"/>
+    <col min="7" max="7" width="7.1640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.1640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.1640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.1640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7" style="31" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.83203125" style="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="M1" s="29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="B2" s="15">
+        <v>0</v>
+      </c>
+      <c r="C2" s="15">
+        <f>LN(B2+0.001)</f>
+        <v>-6.9077552789821368</v>
+      </c>
+      <c r="D2" s="15">
+        <f>IF(B2=0,0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="16">
+        <v>0.43380144492247752</v>
+      </c>
+      <c r="G2" s="15">
+        <v>90</v>
+      </c>
+      <c r="H2" s="15">
+        <v>20</v>
+      </c>
+      <c r="I2" s="15">
+        <v>100</v>
+      </c>
+      <c r="J2" s="15">
+        <v>100</v>
+      </c>
+      <c r="K2" s="15">
+        <v>40</v>
+      </c>
+      <c r="L2" s="31">
+        <f>AVERAGE(G2,H2,K2)</f>
+        <v>50</v>
+      </c>
+      <c r="M2" s="15">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="B3" s="15">
+        <v>0</v>
+      </c>
+      <c r="C3" s="15">
+        <f t="shared" ref="C3:C52" si="0">LN(B3+0.001)</f>
+        <v>-6.9077552789821368</v>
+      </c>
+      <c r="D3" s="15">
+        <f t="shared" ref="D3:D52" si="1">IF(B3=0,0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="16">
+        <v>0.42223267481969268</v>
+      </c>
+      <c r="G3" s="15">
+        <v>70</v>
+      </c>
+      <c r="H3" s="15">
+        <v>90</v>
+      </c>
+      <c r="I3" s="15">
+        <v>90</v>
+      </c>
+      <c r="J3" s="15">
+        <v>90</v>
+      </c>
+      <c r="K3" s="15">
+        <v>80</v>
+      </c>
+      <c r="L3" s="31">
+        <f t="shared" ref="L3:L18" si="2">AVERAGE(G3,H3,K3)</f>
+        <v>80</v>
+      </c>
+      <c r="M3" s="15">
+        <v>13.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="B4" s="15">
+        <v>15</v>
+      </c>
+      <c r="C4" s="15">
+        <f t="shared" si="0"/>
+        <v>2.7081168655467533</v>
+      </c>
+      <c r="D4" s="15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E4" s="15">
+        <v>0</v>
+      </c>
+      <c r="F4" s="16">
+        <v>0.46431654676258999</v>
+      </c>
+      <c r="G4" s="15">
+        <v>60</v>
+      </c>
+      <c r="H4" s="15">
+        <v>80</v>
+      </c>
+      <c r="I4" s="15">
+        <v>70</v>
+      </c>
+      <c r="J4" s="15">
+        <v>90</v>
+      </c>
+      <c r="K4" s="15">
+        <v>70</v>
+      </c>
+      <c r="L4" s="31">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="M4" s="15">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="B5" s="15">
+        <v>8</v>
+      </c>
+      <c r="C5" s="15">
+        <f t="shared" si="0"/>
+        <v>2.079566533867987</v>
+      </c>
+      <c r="D5" s="15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="16">
+        <v>0.53887024608501122</v>
+      </c>
+      <c r="G5" s="15">
+        <v>70</v>
+      </c>
+      <c r="H5" s="15">
+        <v>30</v>
+      </c>
+      <c r="I5" s="15">
+        <v>90</v>
+      </c>
+      <c r="J5" s="15">
+        <v>60</v>
+      </c>
+      <c r="K5" s="15">
+        <v>80</v>
+      </c>
+      <c r="L5" s="31">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="M5" s="20">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="B6" s="15">
+        <v>11</v>
+      </c>
+      <c r="C6" s="15">
+        <f t="shared" si="0"/>
+        <v>2.3979861777572986</v>
+      </c>
+      <c r="D6" s="15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E6" s="15">
+        <v>0</v>
+      </c>
+      <c r="F6" s="16">
+        <v>0.36929046563192902</v>
+      </c>
+      <c r="G6" s="15">
+        <v>70</v>
+      </c>
+      <c r="H6" s="15">
+        <v>50</v>
+      </c>
+      <c r="I6" s="15">
+        <v>90</v>
+      </c>
+      <c r="J6" s="15">
+        <v>90</v>
+      </c>
+      <c r="K6" s="15">
+        <v>90</v>
+      </c>
+      <c r="L6" s="31">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="M6" s="20">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="B7" s="15">
+        <v>3</v>
+      </c>
+      <c r="C7" s="15">
+        <f t="shared" si="0"/>
+        <v>1.0989455664582299</v>
+      </c>
+      <c r="D7" s="15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="16">
+        <v>0.35</v>
+      </c>
+      <c r="G7" s="15">
+        <v>70</v>
+      </c>
+      <c r="H7" s="15">
+        <v>90</v>
+      </c>
+      <c r="I7" s="15">
+        <v>90</v>
+      </c>
+      <c r="J7" s="15">
+        <v>100</v>
+      </c>
+      <c r="K7" s="15">
+        <v>40</v>
+      </c>
+      <c r="L7" s="31">
+        <f t="shared" si="2"/>
+        <v>66.666666666666671</v>
+      </c>
+      <c r="M7" s="20">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="B8" s="15">
+        <v>0</v>
+      </c>
+      <c r="C8" s="15">
+        <f t="shared" si="0"/>
+        <v>-6.9077552789821368</v>
+      </c>
+      <c r="D8" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="16">
+        <v>0.46054442117858213</v>
+      </c>
+      <c r="G8" s="15">
+        <v>40</v>
+      </c>
+      <c r="H8" s="15">
+        <v>60</v>
+      </c>
+      <c r="I8" s="15">
+        <v>100</v>
+      </c>
+      <c r="J8" s="15">
+        <v>100</v>
+      </c>
+      <c r="K8" s="15">
+        <v>80</v>
+      </c>
+      <c r="L8" s="31">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="M8" s="20">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="B9" s="15">
+        <v>0</v>
+      </c>
+      <c r="C9" s="15">
+        <f t="shared" si="0"/>
+        <v>-6.9077552789821368</v>
+      </c>
+      <c r="D9" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="16">
+        <v>0.4539442607463392</v>
+      </c>
+      <c r="G9" s="15">
+        <v>80</v>
+      </c>
+      <c r="H9" s="15">
+        <v>90</v>
+      </c>
+      <c r="I9" s="15">
+        <v>90</v>
+      </c>
+      <c r="J9" s="15">
+        <v>90</v>
+      </c>
+      <c r="K9" s="15">
+        <v>40</v>
+      </c>
+      <c r="L9" s="31">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="M9" s="20">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="B10" s="15">
+        <v>20</v>
+      </c>
+      <c r="C10" s="15">
+        <f t="shared" si="0"/>
+        <v>2.9957822723040328</v>
+      </c>
+      <c r="D10" s="15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="16">
+        <v>0.27963737796373783</v>
+      </c>
+      <c r="G10" s="15">
+        <v>70</v>
+      </c>
+      <c r="H10" s="15">
+        <v>90</v>
+      </c>
+      <c r="I10" s="15">
+        <v>100</v>
+      </c>
+      <c r="J10" s="15">
+        <v>90</v>
+      </c>
+      <c r="K10" s="15">
+        <v>80</v>
+      </c>
+      <c r="L10" s="31">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="M10" s="20">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="B11" s="15">
+        <v>0</v>
+      </c>
+      <c r="C11" s="15">
+        <f t="shared" si="0"/>
+        <v>-6.9077552789821368</v>
+      </c>
+      <c r="D11" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="16">
+        <v>0.35</v>
+      </c>
+      <c r="G11" s="15">
+        <v>90</v>
+      </c>
+      <c r="H11" s="15">
+        <v>90</v>
+      </c>
+      <c r="I11" s="15">
+        <v>90</v>
+      </c>
+      <c r="J11" s="15">
+        <v>100</v>
+      </c>
+      <c r="K11" s="15">
+        <v>80</v>
+      </c>
+      <c r="L11" s="31">
+        <f t="shared" si="2"/>
+        <v>86.666666666666671</v>
+      </c>
+      <c r="M11" s="20">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="B12" s="15">
+        <v>0</v>
+      </c>
+      <c r="C12" s="15">
+        <f t="shared" si="0"/>
+        <v>-6.9077552789821368</v>
+      </c>
+      <c r="D12" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E12" s="15">
+        <v>0</v>
+      </c>
+      <c r="F12" s="16">
+        <v>0.38552361396303902</v>
+      </c>
+      <c r="G12" s="15">
+        <v>90</v>
+      </c>
+      <c r="H12" s="15">
+        <v>80</v>
+      </c>
+      <c r="I12" s="15">
+        <v>100</v>
+      </c>
+      <c r="J12" s="15">
+        <v>90</v>
+      </c>
+      <c r="K12" s="15">
+        <v>90</v>
+      </c>
+      <c r="L12" s="31">
+        <f t="shared" si="2"/>
+        <v>86.666666666666671</v>
+      </c>
+      <c r="M12" s="20">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="B13" s="15">
+        <v>8</v>
+      </c>
+      <c r="C13" s="15">
+        <f t="shared" si="0"/>
+        <v>2.079566533867987</v>
+      </c>
+      <c r="D13" s="15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="16">
+        <v>0.47723201659281606</v>
+      </c>
+      <c r="G13" s="15">
+        <v>90</v>
+      </c>
+      <c r="H13" s="15">
+        <v>80</v>
+      </c>
+      <c r="I13" s="15">
+        <v>90</v>
+      </c>
+      <c r="J13" s="15">
+        <v>100</v>
+      </c>
+      <c r="K13" s="15">
+        <v>60</v>
+      </c>
+      <c r="L13" s="31">
+        <f t="shared" si="2"/>
+        <v>76.666666666666671</v>
+      </c>
+      <c r="M13" s="20">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="B14" s="15">
+        <v>0</v>
+      </c>
+      <c r="C14" s="15">
+        <f t="shared" si="0"/>
+        <v>-6.9077552789821368</v>
+      </c>
+      <c r="D14" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E14" s="15">
+        <v>0</v>
+      </c>
+      <c r="F14" s="16">
+        <v>0.42186580341377283</v>
+      </c>
+      <c r="G14" s="15">
+        <v>100</v>
+      </c>
+      <c r="H14" s="15">
+        <v>100</v>
+      </c>
+      <c r="I14" s="15">
+        <v>100</v>
+      </c>
+      <c r="J14" s="15">
+        <v>100</v>
+      </c>
+      <c r="K14" s="15">
+        <v>90</v>
+      </c>
+      <c r="L14" s="31">
+        <f t="shared" si="2"/>
+        <v>96.666666666666671</v>
+      </c>
+      <c r="M14" s="20">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="B15" s="15">
+        <v>11</v>
+      </c>
+      <c r="C15" s="15">
+        <f t="shared" si="0"/>
+        <v>2.3979861777572986</v>
+      </c>
+      <c r="D15" s="15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E15" s="15">
+        <v>0</v>
+      </c>
+      <c r="F15" s="16">
+        <v>0.43765652951699463</v>
+      </c>
+      <c r="G15" s="15">
+        <v>100</v>
+      </c>
+      <c r="H15" s="15">
+        <v>100</v>
+      </c>
+      <c r="I15" s="15">
+        <v>90</v>
+      </c>
+      <c r="J15" s="15">
+        <v>100</v>
+      </c>
+      <c r="K15" s="15">
+        <v>80</v>
+      </c>
+      <c r="L15" s="31">
+        <f t="shared" si="2"/>
+        <v>93.333333333333329</v>
+      </c>
+      <c r="M15" s="20">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="B16" s="15">
+        <v>0</v>
+      </c>
+      <c r="C16" s="15">
+        <f t="shared" si="0"/>
+        <v>-6.9077552789821368</v>
+      </c>
+      <c r="D16" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="16">
+        <v>0.35168693269395451</v>
+      </c>
+      <c r="G16" s="15">
+        <v>100</v>
+      </c>
+      <c r="H16" s="15">
+        <v>100</v>
+      </c>
+      <c r="I16" s="15">
+        <v>90</v>
+      </c>
+      <c r="J16" s="15">
+        <v>100</v>
+      </c>
+      <c r="K16" s="15">
+        <v>90</v>
+      </c>
+      <c r="L16" s="31">
+        <f t="shared" si="2"/>
+        <v>96.666666666666671</v>
+      </c>
+      <c r="M16" s="20">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="B17" s="15">
+        <v>0</v>
+      </c>
+      <c r="C17" s="15">
+        <f t="shared" si="0"/>
+        <v>-6.9077552789821368</v>
+      </c>
+      <c r="D17" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="16">
+        <v>0.39903746992093503</v>
+      </c>
+      <c r="G17" s="15">
+        <v>100</v>
+      </c>
+      <c r="H17" s="15">
+        <v>90</v>
+      </c>
+      <c r="I17" s="15">
+        <v>80</v>
+      </c>
+      <c r="J17" s="15">
+        <v>100</v>
+      </c>
+      <c r="K17" s="15">
+        <v>100</v>
+      </c>
+      <c r="L17" s="31">
+        <f t="shared" si="2"/>
+        <v>96.666666666666671</v>
+      </c>
+      <c r="M17" s="20">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="B18" s="15">
+        <v>12</v>
+      </c>
+      <c r="C18" s="15">
+        <f t="shared" si="0"/>
+        <v>2.4849899796493045</v>
+      </c>
+      <c r="D18" s="15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E18" s="15">
+        <v>0</v>
+      </c>
+      <c r="F18" s="16">
+        <v>0.34517704517704506</v>
+      </c>
+      <c r="G18" s="15">
+        <v>80</v>
+      </c>
+      <c r="H18" s="15">
+        <v>100</v>
+      </c>
+      <c r="I18" s="15">
+        <v>100</v>
+      </c>
+      <c r="J18" s="15">
+        <v>100</v>
+      </c>
+      <c r="K18" s="15">
+        <v>100</v>
+      </c>
+      <c r="L18" s="31">
+        <f t="shared" si="2"/>
+        <v>93.333333333333329</v>
+      </c>
+      <c r="M18" s="20">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="B19" s="15">
+        <v>0</v>
+      </c>
+      <c r="C19" s="15">
+        <f t="shared" si="0"/>
+        <v>-6.9077552789821368</v>
+      </c>
+      <c r="D19" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="16">
+        <v>0.40032626427406193</v>
+      </c>
+      <c r="G19" s="15">
+        <v>90</v>
+      </c>
+      <c r="H19" s="15">
+        <v>20</v>
+      </c>
+      <c r="I19" s="15">
+        <v>100</v>
+      </c>
+      <c r="J19" s="15">
+        <v>100</v>
+      </c>
+      <c r="K19" s="15">
+        <v>40</v>
+      </c>
+      <c r="L19" s="31">
+        <f>AVERAGE(G19,H19,K19)</f>
+        <v>50</v>
+      </c>
+      <c r="M19" s="20">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="B20" s="15">
+        <v>0</v>
+      </c>
+      <c r="C20" s="15">
+        <f t="shared" si="0"/>
+        <v>-6.9077552789821368</v>
+      </c>
+      <c r="D20" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E20" s="15">
+        <v>0</v>
+      </c>
+      <c r="F20" s="16">
+        <v>0.37900023359028256</v>
+      </c>
+      <c r="G20" s="15">
+        <v>70</v>
+      </c>
+      <c r="H20" s="15">
+        <v>90</v>
+      </c>
+      <c r="I20" s="15">
+        <v>90</v>
+      </c>
+      <c r="J20" s="15">
+        <v>90</v>
+      </c>
+      <c r="K20" s="15">
+        <v>80</v>
+      </c>
+      <c r="L20" s="31">
+        <f t="shared" ref="L20:L35" si="3">AVERAGE(G20,H20,K20)</f>
+        <v>80</v>
+      </c>
+      <c r="M20" s="20">
+        <v>13.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="B21" s="15">
+        <v>28</v>
+      </c>
+      <c r="C21" s="15">
+        <f t="shared" si="0"/>
+        <v>3.3322402238231783</v>
+      </c>
+      <c r="D21" s="15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F21" s="16">
+        <v>0.41577181208053687</v>
+      </c>
+      <c r="G21" s="15">
+        <v>60</v>
+      </c>
+      <c r="H21" s="15">
+        <v>80</v>
+      </c>
+      <c r="I21" s="15">
+        <v>70</v>
+      </c>
+      <c r="J21" s="15">
+        <v>90</v>
+      </c>
+      <c r="K21" s="15">
+        <v>70</v>
+      </c>
+      <c r="L21" s="31">
+        <f t="shared" si="3"/>
+        <v>70</v>
+      </c>
+      <c r="M21" s="20">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="B22" s="15">
+        <v>15</v>
+      </c>
+      <c r="C22" s="15">
+        <f t="shared" si="0"/>
+        <v>2.7081168655467533</v>
+      </c>
+      <c r="D22" s="15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F22" s="16">
+        <v>0.45123674911660783</v>
+      </c>
+      <c r="G22" s="15">
+        <v>70</v>
+      </c>
+      <c r="H22" s="15">
+        <v>30</v>
+      </c>
+      <c r="I22" s="15">
+        <v>90</v>
+      </c>
+      <c r="J22" s="15">
+        <v>60</v>
+      </c>
+      <c r="K22" s="15">
+        <v>80</v>
+      </c>
+      <c r="L22" s="31">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="M22" s="20">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="B23" s="15">
+        <v>44</v>
+      </c>
+      <c r="C23" s="15">
+        <f t="shared" si="0"/>
+        <v>3.7842123609327278</v>
+      </c>
+      <c r="D23" s="15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E23" s="15">
+        <v>0</v>
+      </c>
+      <c r="F23" s="16">
+        <v>0.31794248683677606</v>
+      </c>
+      <c r="G23" s="15">
+        <v>70</v>
+      </c>
+      <c r="H23" s="15">
+        <v>50</v>
+      </c>
+      <c r="I23" s="15">
+        <v>90</v>
+      </c>
+      <c r="J23" s="15">
+        <v>90</v>
+      </c>
+      <c r="K23" s="15">
+        <v>90</v>
+      </c>
+      <c r="L23" s="31">
+        <f t="shared" si="3"/>
+        <v>70</v>
+      </c>
+      <c r="M23" s="20">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="B24" s="15">
+        <v>0</v>
+      </c>
+      <c r="C24" s="15">
+        <f t="shared" si="0"/>
+        <v>-6.9077552789821368</v>
+      </c>
+      <c r="D24" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" s="16">
+        <v>0.43278185603155483</v>
+      </c>
+      <c r="G24" s="15">
+        <v>70</v>
+      </c>
+      <c r="H24" s="15">
+        <v>90</v>
+      </c>
+      <c r="I24" s="15">
+        <v>90</v>
+      </c>
+      <c r="J24" s="15">
+        <v>100</v>
+      </c>
+      <c r="K24" s="15">
+        <v>40</v>
+      </c>
+      <c r="L24" s="31">
+        <f t="shared" si="3"/>
+        <v>66.666666666666671</v>
+      </c>
+      <c r="M24" s="20">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="B25" s="15">
+        <v>0</v>
+      </c>
+      <c r="C25" s="15">
+        <f t="shared" si="0"/>
+        <v>-6.9077552789821368</v>
+      </c>
+      <c r="D25" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F25" s="16">
+        <v>0.40381439894319682</v>
+      </c>
+      <c r="G25" s="15">
+        <v>40</v>
+      </c>
+      <c r="H25" s="15">
+        <v>60</v>
+      </c>
+      <c r="I25" s="15">
+        <v>100</v>
+      </c>
+      <c r="J25" s="15">
+        <v>100</v>
+      </c>
+      <c r="K25" s="15">
+        <v>80</v>
+      </c>
+      <c r="L25" s="31">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="M25" s="20">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="B26" s="15">
+        <v>0</v>
+      </c>
+      <c r="C26" s="15">
+        <f t="shared" si="0"/>
+        <v>-6.9077552789821368</v>
+      </c>
+      <c r="D26" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F26" s="16">
+        <v>0.23604106628242064</v>
+      </c>
+      <c r="G26" s="15">
+        <v>80</v>
+      </c>
+      <c r="H26" s="15">
+        <v>90</v>
+      </c>
+      <c r="I26" s="15">
+        <v>90</v>
+      </c>
+      <c r="J26" s="15">
+        <v>90</v>
+      </c>
+      <c r="K26" s="15">
+        <v>40</v>
+      </c>
+      <c r="L26" s="31">
+        <f t="shared" si="3"/>
+        <v>70</v>
+      </c>
+      <c r="M26" s="20">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="B27" s="15">
+        <v>12</v>
+      </c>
+      <c r="C27" s="15">
+        <f t="shared" si="0"/>
+        <v>2.4849899796493045</v>
+      </c>
+      <c r="D27" s="15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E27" s="15">
+        <v>0</v>
+      </c>
+      <c r="F27" s="16">
+        <v>0.39749423013517965</v>
+      </c>
+      <c r="G27" s="15">
+        <v>70</v>
+      </c>
+      <c r="H27" s="15">
+        <v>90</v>
+      </c>
+      <c r="I27" s="15">
+        <v>100</v>
+      </c>
+      <c r="J27" s="15">
+        <v>90</v>
+      </c>
+      <c r="K27" s="15">
+        <v>80</v>
+      </c>
+      <c r="L27" s="31">
+        <f t="shared" si="3"/>
+        <v>80</v>
+      </c>
+      <c r="M27" s="20">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="B28" s="15">
+        <v>0</v>
+      </c>
+      <c r="C28" s="15">
+        <f t="shared" si="0"/>
+        <v>-6.9077552789821368</v>
+      </c>
+      <c r="D28" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F28" s="16">
+        <v>0.44650666666666666</v>
+      </c>
+      <c r="G28" s="15">
+        <v>90</v>
+      </c>
+      <c r="H28" s="15">
+        <v>90</v>
+      </c>
+      <c r="I28" s="15">
+        <v>90</v>
+      </c>
+      <c r="J28" s="15">
+        <v>100</v>
+      </c>
+      <c r="K28" s="15">
+        <v>80</v>
+      </c>
+      <c r="L28" s="31">
+        <f t="shared" si="3"/>
+        <v>86.666666666666671</v>
+      </c>
+      <c r="M28" s="20">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="B29" s="15">
+        <v>0</v>
+      </c>
+      <c r="C29" s="15">
+        <f t="shared" si="0"/>
+        <v>-6.9077552789821368</v>
+      </c>
+      <c r="D29" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E29" s="15">
+        <v>0</v>
+      </c>
+      <c r="F29" s="16">
+        <v>0.43278185603155483</v>
+      </c>
+      <c r="G29" s="15">
+        <v>90</v>
+      </c>
+      <c r="H29" s="15">
+        <v>80</v>
+      </c>
+      <c r="I29" s="15">
+        <v>100</v>
+      </c>
+      <c r="J29" s="15">
+        <v>90</v>
+      </c>
+      <c r="K29" s="15">
+        <v>90</v>
+      </c>
+      <c r="L29" s="31">
+        <f t="shared" si="3"/>
+        <v>86.666666666666671</v>
+      </c>
+      <c r="M29" s="20">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="B30" s="15">
+        <v>13</v>
+      </c>
+      <c r="C30" s="15">
+        <f t="shared" si="0"/>
+        <v>2.5650262775800314</v>
+      </c>
+      <c r="D30" s="15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F30" s="16">
+        <v>0.40480961923847691</v>
+      </c>
+      <c r="G30" s="15">
+        <v>90</v>
+      </c>
+      <c r="H30" s="15">
+        <v>80</v>
+      </c>
+      <c r="I30" s="15">
+        <v>90</v>
+      </c>
+      <c r="J30" s="15">
+        <v>100</v>
+      </c>
+      <c r="K30" s="15">
+        <v>60</v>
+      </c>
+      <c r="L30" s="31">
+        <f t="shared" si="3"/>
+        <v>76.666666666666671</v>
+      </c>
+      <c r="M30" s="20">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="B31" s="15">
+        <v>0</v>
+      </c>
+      <c r="C31" s="15">
+        <f t="shared" si="0"/>
+        <v>-6.9077552789821368</v>
+      </c>
+      <c r="D31" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E31" s="15">
+        <v>0</v>
+      </c>
+      <c r="F31" s="16">
+        <v>0.415685987866384</v>
+      </c>
+      <c r="G31" s="15">
+        <v>100</v>
+      </c>
+      <c r="H31" s="15">
+        <v>100</v>
+      </c>
+      <c r="I31" s="15">
+        <v>100</v>
+      </c>
+      <c r="J31" s="15">
+        <v>100</v>
+      </c>
+      <c r="K31" s="15">
+        <v>90</v>
+      </c>
+      <c r="L31" s="31">
+        <f t="shared" si="3"/>
+        <v>96.666666666666671</v>
+      </c>
+      <c r="M31" s="20">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="B32" s="15">
+        <v>14</v>
+      </c>
+      <c r="C32" s="15">
+        <f t="shared" si="0"/>
+        <v>2.6391287556357881</v>
+      </c>
+      <c r="D32" s="15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E32" s="15">
+        <v>0</v>
+      </c>
+      <c r="F32" s="16">
+        <v>0.41123247473100755</v>
+      </c>
+      <c r="G32" s="15">
+        <v>100</v>
+      </c>
+      <c r="H32" s="15">
+        <v>100</v>
+      </c>
+      <c r="I32" s="15">
+        <v>90</v>
+      </c>
+      <c r="J32" s="15">
+        <v>100</v>
+      </c>
+      <c r="K32" s="15">
+        <v>80</v>
+      </c>
+      <c r="L32" s="31">
+        <f t="shared" si="3"/>
+        <v>93.333333333333329</v>
+      </c>
+      <c r="M32" s="20">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="B33" s="15">
+        <v>0</v>
+      </c>
+      <c r="C33" s="15">
+        <f t="shared" si="0"/>
+        <v>-6.9077552789821368</v>
+      </c>
+      <c r="D33" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E33" s="15">
+        <v>0</v>
+      </c>
+      <c r="F33" s="16">
+        <v>0.30132343447385412</v>
+      </c>
+      <c r="G33" s="15">
+        <v>100</v>
+      </c>
+      <c r="H33" s="15">
+        <v>100</v>
+      </c>
+      <c r="I33" s="15">
+        <v>90</v>
+      </c>
+      <c r="J33" s="15">
+        <v>100</v>
+      </c>
+      <c r="K33" s="15">
+        <v>90</v>
+      </c>
+      <c r="L33" s="31">
+        <f t="shared" si="3"/>
+        <v>96.666666666666671</v>
+      </c>
+      <c r="M33" s="20">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="B34" s="15">
+        <v>0</v>
+      </c>
+      <c r="C34" s="15">
+        <f t="shared" si="0"/>
+        <v>-6.9077552789821368</v>
+      </c>
+      <c r="D34" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E34" s="15">
+        <v>0</v>
+      </c>
+      <c r="F34" s="16">
+        <v>0.3078115313081215</v>
+      </c>
+      <c r="G34" s="15">
+        <v>100</v>
+      </c>
+      <c r="H34" s="15">
+        <v>90</v>
+      </c>
+      <c r="I34" s="15">
+        <v>80</v>
+      </c>
+      <c r="J34" s="15">
+        <v>100</v>
+      </c>
+      <c r="K34" s="15">
+        <v>100</v>
+      </c>
+      <c r="L34" s="31">
+        <f t="shared" si="3"/>
+        <v>96.666666666666671</v>
+      </c>
+      <c r="M34" s="20">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="B35" s="15">
+        <v>15</v>
+      </c>
+      <c r="C35" s="15">
+        <f t="shared" si="0"/>
+        <v>2.7081168655467533</v>
+      </c>
+      <c r="D35" s="15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E35" s="15">
+        <v>0</v>
+      </c>
+      <c r="F35" s="16">
+        <v>0.35321692253603648</v>
+      </c>
+      <c r="G35" s="15">
+        <v>80</v>
+      </c>
+      <c r="H35" s="15">
+        <v>100</v>
+      </c>
+      <c r="I35" s="15">
+        <v>100</v>
+      </c>
+      <c r="J35" s="15">
+        <v>100</v>
+      </c>
+      <c r="K35" s="15">
+        <v>100</v>
+      </c>
+      <c r="L35" s="31">
+        <f t="shared" si="3"/>
+        <v>93.333333333333329</v>
+      </c>
+      <c r="M35" s="20">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="15">
+        <f>0.5+A19</f>
+        <v>0.75</v>
+      </c>
+      <c r="B36" s="15">
+        <v>0</v>
+      </c>
+      <c r="C36" s="15">
+        <f t="shared" si="0"/>
+        <v>-6.9077552789821368</v>
+      </c>
+      <c r="D36" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F36" s="16">
+        <v>0.25809840658378569</v>
+      </c>
+      <c r="G36" s="15">
+        <v>90</v>
+      </c>
+      <c r="H36" s="15">
+        <v>20</v>
+      </c>
+      <c r="I36" s="15">
+        <v>100</v>
+      </c>
+      <c r="J36" s="15">
+        <v>100</v>
+      </c>
+      <c r="K36" s="15">
+        <v>40</v>
+      </c>
+      <c r="L36" s="31">
+        <f>AVERAGE(G36,H36,K36)</f>
+        <v>50</v>
+      </c>
+      <c r="M36" s="15">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="15">
+        <f t="shared" ref="A37:A52" si="4">0.5+A20</f>
+        <v>0.75</v>
+      </c>
+      <c r="B37" s="15">
+        <v>0</v>
+      </c>
+      <c r="C37" s="15">
+        <f t="shared" si="0"/>
+        <v>-6.9077552789821368</v>
+      </c>
+      <c r="D37" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E37" s="15">
+        <v>0</v>
+      </c>
+      <c r="F37" s="16">
+        <v>0.11742526259089683</v>
+      </c>
+      <c r="G37" s="15">
+        <v>70</v>
+      </c>
+      <c r="H37" s="15">
+        <v>90</v>
+      </c>
+      <c r="I37" s="15">
+        <v>90</v>
+      </c>
+      <c r="J37" s="15">
+        <v>90</v>
+      </c>
+      <c r="K37" s="15">
+        <v>80</v>
+      </c>
+      <c r="L37" s="31">
+        <f t="shared" ref="L37:L52" si="5">AVERAGE(G37,H37,K37)</f>
+        <v>80</v>
+      </c>
+      <c r="M37" s="15">
+        <v>13.9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="15">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="B38" s="15">
+        <v>0</v>
+      </c>
+      <c r="C38" s="15">
+        <f t="shared" si="0"/>
+        <v>-6.9077552789821368</v>
+      </c>
+      <c r="D38" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E38" s="15">
+        <v>0</v>
+      </c>
+      <c r="F38" s="16">
+        <v>0.23132451055452269</v>
+      </c>
+      <c r="G38" s="15">
+        <v>60</v>
+      </c>
+      <c r="H38" s="15">
+        <v>80</v>
+      </c>
+      <c r="I38" s="15">
+        <v>70</v>
+      </c>
+      <c r="J38" s="15">
+        <v>90</v>
+      </c>
+      <c r="K38" s="15">
+        <v>70</v>
+      </c>
+      <c r="L38" s="31">
+        <f t="shared" si="5"/>
+        <v>70</v>
+      </c>
+      <c r="M38" s="15">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="15">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="B39" s="15">
+        <v>1</v>
+      </c>
+      <c r="C39" s="15">
+        <f t="shared" si="0"/>
+        <v>9.9950033308342321E-4</v>
+      </c>
+      <c r="D39" s="15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E39" s="15">
+        <v>0</v>
+      </c>
+      <c r="F39" s="16">
+        <v>0.38323477539163808</v>
+      </c>
+      <c r="G39" s="15">
+        <v>70</v>
+      </c>
+      <c r="H39" s="15">
+        <v>30</v>
+      </c>
+      <c r="I39" s="15">
+        <v>90</v>
+      </c>
+      <c r="J39" s="15">
+        <v>60</v>
+      </c>
+      <c r="K39" s="15">
+        <v>80</v>
+      </c>
+      <c r="L39" s="31">
+        <f t="shared" si="5"/>
+        <v>60</v>
+      </c>
+      <c r="M39" s="20">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40" s="15">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="B40" s="15">
+        <v>0</v>
+      </c>
+      <c r="C40" s="15">
+        <f t="shared" si="0"/>
+        <v>-6.9077552789821368</v>
+      </c>
+      <c r="D40" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E40" s="15">
+        <v>0</v>
+      </c>
+      <c r="F40" s="16">
+        <v>0.29475043029259906</v>
+      </c>
+      <c r="G40" s="15">
+        <v>70</v>
+      </c>
+      <c r="H40" s="15">
+        <v>50</v>
+      </c>
+      <c r="I40" s="15">
+        <v>90</v>
+      </c>
+      <c r="J40" s="15">
+        <v>90</v>
+      </c>
+      <c r="K40" s="15">
+        <v>90</v>
+      </c>
+      <c r="L40" s="31">
+        <f t="shared" si="5"/>
+        <v>70</v>
+      </c>
+      <c r="M40" s="20">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41" s="15">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="B41" s="15">
+        <v>0</v>
+      </c>
+      <c r="C41" s="15">
+        <f t="shared" si="0"/>
+        <v>-6.9077552789821368</v>
+      </c>
+      <c r="D41" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E41" s="15">
+        <v>0</v>
+      </c>
+      <c r="F41" s="16">
+        <v>0.26349390597794553</v>
+      </c>
+      <c r="G41" s="15">
+        <v>70</v>
+      </c>
+      <c r="H41" s="15">
+        <v>90</v>
+      </c>
+      <c r="I41" s="15">
+        <v>90</v>
+      </c>
+      <c r="J41" s="15">
+        <v>100</v>
+      </c>
+      <c r="K41" s="15">
+        <v>40</v>
+      </c>
+      <c r="L41" s="31">
+        <f t="shared" si="5"/>
+        <v>66.666666666666671</v>
+      </c>
+      <c r="M41" s="20">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" s="15">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="B42" s="15">
+        <v>0</v>
+      </c>
+      <c r="C42" s="15">
+        <f t="shared" si="0"/>
+        <v>-6.9077552789821368</v>
+      </c>
+      <c r="D42" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E42" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F42" s="16">
+        <v>0.27677564825253659</v>
+      </c>
+      <c r="G42" s="15">
+        <v>40</v>
+      </c>
+      <c r="H42" s="15">
+        <v>60</v>
+      </c>
+      <c r="I42" s="15">
+        <v>100</v>
+      </c>
+      <c r="J42" s="15">
+        <v>100</v>
+      </c>
+      <c r="K42" s="15">
+        <v>80</v>
+      </c>
+      <c r="L42" s="31">
+        <f t="shared" si="5"/>
+        <v>60</v>
+      </c>
+      <c r="M42" s="20">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" s="15">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="B43" s="15">
+        <v>0</v>
+      </c>
+      <c r="C43" s="15">
+        <f t="shared" si="0"/>
+        <v>-6.9077552789821368</v>
+      </c>
+      <c r="D43" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E43" s="15">
+        <v>0</v>
+      </c>
+      <c r="F43" s="16">
+        <v>0.27963737796373783</v>
+      </c>
+      <c r="G43" s="15">
+        <v>80</v>
+      </c>
+      <c r="H43" s="15">
+        <v>90</v>
+      </c>
+      <c r="I43" s="15">
+        <v>90</v>
+      </c>
+      <c r="J43" s="15">
+        <v>90</v>
+      </c>
+      <c r="K43" s="15">
+        <v>40</v>
+      </c>
+      <c r="L43" s="31">
+        <f t="shared" si="5"/>
+        <v>70</v>
+      </c>
+      <c r="M43" s="20">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="A44" s="15">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="B44" s="15">
+        <v>0</v>
+      </c>
+      <c r="C44" s="15">
+        <f t="shared" si="0"/>
+        <v>-6.9077552789821368</v>
+      </c>
+      <c r="D44" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E44" s="15">
+        <v>0</v>
+      </c>
+      <c r="F44" s="16">
+        <v>0.29137630662020902</v>
+      </c>
+      <c r="G44" s="15">
+        <v>70</v>
+      </c>
+      <c r="H44" s="15">
+        <v>90</v>
+      </c>
+      <c r="I44" s="15">
+        <v>100</v>
+      </c>
+      <c r="J44" s="15">
+        <v>90</v>
+      </c>
+      <c r="K44" s="15">
+        <v>80</v>
+      </c>
+      <c r="L44" s="31">
+        <f t="shared" si="5"/>
+        <v>80</v>
+      </c>
+      <c r="M44" s="20">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="A45" s="15">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="B45" s="15">
+        <v>0</v>
+      </c>
+      <c r="C45" s="15">
+        <f t="shared" si="0"/>
+        <v>-6.9077552789821368</v>
+      </c>
+      <c r="D45" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E45" s="15">
+        <v>0</v>
+      </c>
+      <c r="F45" s="16">
+        <v>0.40324158166829677</v>
+      </c>
+      <c r="G45" s="15">
+        <v>90</v>
+      </c>
+      <c r="H45" s="15">
+        <v>90</v>
+      </c>
+      <c r="I45" s="15">
+        <v>90</v>
+      </c>
+      <c r="J45" s="15">
+        <v>100</v>
+      </c>
+      <c r="K45" s="15">
+        <v>80</v>
+      </c>
+      <c r="L45" s="31">
+        <f t="shared" si="5"/>
+        <v>86.666666666666671</v>
+      </c>
+      <c r="M45" s="20">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="A46" s="15">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="B46" s="15">
+        <v>0</v>
+      </c>
+      <c r="C46" s="15">
+        <f t="shared" si="0"/>
+        <v>-6.9077552789821368</v>
+      </c>
+      <c r="D46" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E46" s="15">
+        <v>0</v>
+      </c>
+      <c r="F46" s="16">
+        <v>0.38038679840235445</v>
+      </c>
+      <c r="G46" s="15">
+        <v>90</v>
+      </c>
+      <c r="H46" s="15">
+        <v>80</v>
+      </c>
+      <c r="I46" s="15">
+        <v>100</v>
+      </c>
+      <c r="J46" s="15">
+        <v>90</v>
+      </c>
+      <c r="K46" s="15">
+        <v>90</v>
+      </c>
+      <c r="L46" s="31">
+        <f t="shared" si="5"/>
+        <v>86.666666666666671</v>
+      </c>
+      <c r="M46" s="20">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
+      <c r="A47" s="15">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="B47" s="15">
+        <v>0</v>
+      </c>
+      <c r="C47" s="15">
+        <f t="shared" si="0"/>
+        <v>-6.9077552789821368</v>
+      </c>
+      <c r="D47" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E47" s="15">
+        <v>0</v>
+      </c>
+      <c r="F47" s="16">
+        <v>0.24292995725090433</v>
+      </c>
+      <c r="G47" s="15">
+        <v>90</v>
+      </c>
+      <c r="H47" s="15">
+        <v>80</v>
+      </c>
+      <c r="I47" s="15">
+        <v>90</v>
+      </c>
+      <c r="J47" s="15">
+        <v>100</v>
+      </c>
+      <c r="K47" s="15">
+        <v>60</v>
+      </c>
+      <c r="L47" s="31">
+        <f t="shared" si="5"/>
+        <v>76.666666666666671</v>
+      </c>
+      <c r="M47" s="20">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="A48" s="15">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="B48" s="15">
+        <v>0</v>
+      </c>
+      <c r="C48" s="15">
+        <f t="shared" si="0"/>
+        <v>-6.9077552789821368</v>
+      </c>
+      <c r="D48" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E48" s="15">
+        <v>0</v>
+      </c>
+      <c r="F48" s="16">
+        <v>0.169047619047619</v>
+      </c>
+      <c r="G48" s="15">
+        <v>100</v>
+      </c>
+      <c r="H48" s="15">
+        <v>100</v>
+      </c>
+      <c r="I48" s="15">
+        <v>100</v>
+      </c>
+      <c r="J48" s="15">
+        <v>100</v>
+      </c>
+      <c r="K48" s="15">
+        <v>90</v>
+      </c>
+      <c r="L48" s="31">
+        <f t="shared" si="5"/>
+        <v>96.666666666666671</v>
+      </c>
+      <c r="M48" s="20">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13">
+      <c r="A49" s="15">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="B49" s="15">
+        <v>1</v>
+      </c>
+      <c r="C49" s="15">
+        <f t="shared" si="0"/>
+        <v>9.9950033308342321E-4</v>
+      </c>
+      <c r="D49" s="15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E49" s="15">
+        <v>0</v>
+      </c>
+      <c r="F49" s="16">
+        <v>0.27698226116691604</v>
+      </c>
+      <c r="G49" s="15">
+        <v>100</v>
+      </c>
+      <c r="H49" s="15">
+        <v>100</v>
+      </c>
+      <c r="I49" s="15">
+        <v>90</v>
+      </c>
+      <c r="J49" s="15">
+        <v>100</v>
+      </c>
+      <c r="K49" s="15">
+        <v>80</v>
+      </c>
+      <c r="L49" s="31">
+        <f t="shared" si="5"/>
+        <v>93.333333333333329</v>
+      </c>
+      <c r="M49" s="20">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13">
+      <c r="A50" s="15">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="B50" s="15">
+        <v>0</v>
+      </c>
+      <c r="C50" s="15">
+        <f t="shared" si="0"/>
+        <v>-6.9077552789821368</v>
+      </c>
+      <c r="D50" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E50" s="15">
+        <v>0</v>
+      </c>
+      <c r="F50" s="16">
+        <v>0.25380258899676367</v>
+      </c>
+      <c r="G50" s="15">
+        <v>100</v>
+      </c>
+      <c r="H50" s="15">
+        <v>100</v>
+      </c>
+      <c r="I50" s="15">
+        <v>90</v>
+      </c>
+      <c r="J50" s="15">
+        <v>100</v>
+      </c>
+      <c r="K50" s="15">
+        <v>90</v>
+      </c>
+      <c r="L50" s="31">
+        <f t="shared" si="5"/>
+        <v>96.666666666666671</v>
+      </c>
+      <c r="M50" s="20">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13">
+      <c r="A51" s="15">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="B51" s="15">
+        <v>0</v>
+      </c>
+      <c r="C51" s="15">
+        <f t="shared" si="0"/>
+        <v>-6.9077552789821368</v>
+      </c>
+      <c r="D51" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E51" s="15">
+        <v>0</v>
+      </c>
+      <c r="F51" s="16">
+        <v>0.12557523357969599</v>
+      </c>
+      <c r="G51" s="15">
+        <v>100</v>
+      </c>
+      <c r="H51" s="15">
+        <v>90</v>
+      </c>
+      <c r="I51" s="15">
+        <v>80</v>
+      </c>
+      <c r="J51" s="15">
+        <v>100</v>
+      </c>
+      <c r="K51" s="15">
+        <v>100</v>
+      </c>
+      <c r="L51" s="31">
+        <f t="shared" si="5"/>
+        <v>96.666666666666671</v>
+      </c>
+      <c r="M51" s="20">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13">
+      <c r="A52" s="15">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="B52" s="15">
+        <v>0</v>
+      </c>
+      <c r="C52" s="15">
+        <f t="shared" si="0"/>
+        <v>-6.9077552789821368</v>
+      </c>
+      <c r="D52" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E52" s="15">
+        <v>0</v>
+      </c>
+      <c r="F52" s="16">
+        <v>0.39540306462358427</v>
+      </c>
+      <c r="G52" s="15">
+        <v>80</v>
+      </c>
+      <c r="H52" s="15">
+        <v>100</v>
+      </c>
+      <c r="I52" s="15">
+        <v>100</v>
+      </c>
+      <c r="J52" s="15">
+        <v>100</v>
+      </c>
+      <c r="K52" s="15">
+        <v>100</v>
+      </c>
+      <c r="L52" s="31">
+        <f t="shared" si="5"/>
+        <v>93.333333333333329</v>
+      </c>
+      <c r="M52" s="20">
+        <v>1.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:Y21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD19"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2367,12 +4708,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -3451,7 +5792,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AG1003"/>
@@ -17749,7 +20090,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H25"/>
@@ -18453,7 +20794,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:Z41"/>
@@ -20963,2351 +23304,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet7" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:M52"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:M1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="8.33203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5" style="15" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.83203125" style="15" customWidth="1"/>
-    <col min="7" max="7" width="7.1640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.1640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.1640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.1640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.5" style="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7" style="31" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.83203125" style="15" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13">
-      <c r="A1" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="C1" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="D1" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="E1" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="G1" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="M1" s="29" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="B2" s="15">
-        <v>0</v>
-      </c>
-      <c r="C2" s="15">
-        <f>LN(B2+0.001)</f>
-        <v>-6.9077552789821368</v>
-      </c>
-      <c r="D2" s="15">
-        <f>IF(B2=0,0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" s="16">
-        <v>0.43380144492247752</v>
-      </c>
-      <c r="G2" s="15">
-        <v>90</v>
-      </c>
-      <c r="H2" s="15">
-        <v>20</v>
-      </c>
-      <c r="I2" s="15">
-        <v>100</v>
-      </c>
-      <c r="J2" s="15">
-        <v>100</v>
-      </c>
-      <c r="K2" s="15">
-        <v>40</v>
-      </c>
-      <c r="L2" s="31">
-        <f>AVERAGE(G2,H2,K2)</f>
-        <v>50</v>
-      </c>
-      <c r="M2" s="15">
-        <v>3.9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="B3" s="15">
-        <v>0</v>
-      </c>
-      <c r="C3" s="15">
-        <f t="shared" ref="C3:C52" si="0">LN(B3+0.001)</f>
-        <v>-6.9077552789821368</v>
-      </c>
-      <c r="D3" s="15">
-        <f t="shared" ref="D3:D52" si="1">IF(B3=0,0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="16">
-        <v>0.42223267481969268</v>
-      </c>
-      <c r="G3" s="15">
-        <v>70</v>
-      </c>
-      <c r="H3" s="15">
-        <v>90</v>
-      </c>
-      <c r="I3" s="15">
-        <v>90</v>
-      </c>
-      <c r="J3" s="15">
-        <v>90</v>
-      </c>
-      <c r="K3" s="15">
-        <v>80</v>
-      </c>
-      <c r="L3" s="31">
-        <f t="shared" ref="L3:L18" si="2">AVERAGE(G3,H3,K3)</f>
-        <v>80</v>
-      </c>
-      <c r="M3" s="15">
-        <v>13.9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="B4" s="15">
-        <v>15</v>
-      </c>
-      <c r="C4" s="15">
-        <f t="shared" si="0"/>
-        <v>2.7081168655467533</v>
-      </c>
-      <c r="D4" s="15">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E4" s="15">
-        <v>0</v>
-      </c>
-      <c r="F4" s="16">
-        <v>0.46431654676258999</v>
-      </c>
-      <c r="G4" s="15">
-        <v>60</v>
-      </c>
-      <c r="H4" s="15">
-        <v>80</v>
-      </c>
-      <c r="I4" s="15">
-        <v>70</v>
-      </c>
-      <c r="J4" s="15">
-        <v>90</v>
-      </c>
-      <c r="K4" s="15">
-        <v>70</v>
-      </c>
-      <c r="L4" s="31">
-        <f t="shared" si="2"/>
-        <v>70</v>
-      </c>
-      <c r="M4" s="15">
-        <v>3.1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="B5" s="15">
-        <v>8</v>
-      </c>
-      <c r="C5" s="15">
-        <f t="shared" si="0"/>
-        <v>2.079566533867987</v>
-      </c>
-      <c r="D5" s="15">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="16">
-        <v>0.53887024608501122</v>
-      </c>
-      <c r="G5" s="15">
-        <v>70</v>
-      </c>
-      <c r="H5" s="15">
-        <v>30</v>
-      </c>
-      <c r="I5" s="15">
-        <v>90</v>
-      </c>
-      <c r="J5" s="15">
-        <v>60</v>
-      </c>
-      <c r="K5" s="15">
-        <v>80</v>
-      </c>
-      <c r="L5" s="31">
-        <f t="shared" si="2"/>
-        <v>60</v>
-      </c>
-      <c r="M5" s="20">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="B6" s="15">
-        <v>11</v>
-      </c>
-      <c r="C6" s="15">
-        <f t="shared" si="0"/>
-        <v>2.3979861777572986</v>
-      </c>
-      <c r="D6" s="15">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E6" s="15">
-        <v>0</v>
-      </c>
-      <c r="F6" s="16">
-        <v>0.36929046563192902</v>
-      </c>
-      <c r="G6" s="15">
-        <v>70</v>
-      </c>
-      <c r="H6" s="15">
-        <v>50</v>
-      </c>
-      <c r="I6" s="15">
-        <v>90</v>
-      </c>
-      <c r="J6" s="15">
-        <v>90</v>
-      </c>
-      <c r="K6" s="15">
-        <v>90</v>
-      </c>
-      <c r="L6" s="31">
-        <f t="shared" si="2"/>
-        <v>70</v>
-      </c>
-      <c r="M6" s="20">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="B7" s="15">
-        <v>3</v>
-      </c>
-      <c r="C7" s="15">
-        <f t="shared" si="0"/>
-        <v>1.0989455664582299</v>
-      </c>
-      <c r="D7" s="15">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" s="16">
-        <v>0.35</v>
-      </c>
-      <c r="G7" s="15">
-        <v>70</v>
-      </c>
-      <c r="H7" s="15">
-        <v>90</v>
-      </c>
-      <c r="I7" s="15">
-        <v>90</v>
-      </c>
-      <c r="J7" s="15">
-        <v>100</v>
-      </c>
-      <c r="K7" s="15">
-        <v>40</v>
-      </c>
-      <c r="L7" s="31">
-        <f t="shared" si="2"/>
-        <v>66.666666666666671</v>
-      </c>
-      <c r="M7" s="20">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="B8" s="15">
-        <v>0</v>
-      </c>
-      <c r="C8" s="15">
-        <f t="shared" si="0"/>
-        <v>-6.9077552789821368</v>
-      </c>
-      <c r="D8" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="16">
-        <v>0.46054442117858213</v>
-      </c>
-      <c r="G8" s="15">
-        <v>40</v>
-      </c>
-      <c r="H8" s="15">
-        <v>60</v>
-      </c>
-      <c r="I8" s="15">
-        <v>100</v>
-      </c>
-      <c r="J8" s="15">
-        <v>100</v>
-      </c>
-      <c r="K8" s="15">
-        <v>80</v>
-      </c>
-      <c r="L8" s="31">
-        <f t="shared" si="2"/>
-        <v>60</v>
-      </c>
-      <c r="M8" s="20">
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="B9" s="15">
-        <v>0</v>
-      </c>
-      <c r="C9" s="15">
-        <f t="shared" si="0"/>
-        <v>-6.9077552789821368</v>
-      </c>
-      <c r="D9" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="16">
-        <v>0.4539442607463392</v>
-      </c>
-      <c r="G9" s="15">
-        <v>80</v>
-      </c>
-      <c r="H9" s="15">
-        <v>90</v>
-      </c>
-      <c r="I9" s="15">
-        <v>90</v>
-      </c>
-      <c r="J9" s="15">
-        <v>90</v>
-      </c>
-      <c r="K9" s="15">
-        <v>40</v>
-      </c>
-      <c r="L9" s="31">
-        <f t="shared" si="2"/>
-        <v>70</v>
-      </c>
-      <c r="M9" s="20">
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="B10" s="15">
-        <v>20</v>
-      </c>
-      <c r="C10" s="15">
-        <f t="shared" si="0"/>
-        <v>2.9957822723040328</v>
-      </c>
-      <c r="D10" s="15">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="16">
-        <v>0.27963737796373783</v>
-      </c>
-      <c r="G10" s="15">
-        <v>70</v>
-      </c>
-      <c r="H10" s="15">
-        <v>90</v>
-      </c>
-      <c r="I10" s="15">
-        <v>100</v>
-      </c>
-      <c r="J10" s="15">
-        <v>90</v>
-      </c>
-      <c r="K10" s="15">
-        <v>80</v>
-      </c>
-      <c r="L10" s="31">
-        <f t="shared" si="2"/>
-        <v>80</v>
-      </c>
-      <c r="M10" s="20">
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="B11" s="15">
-        <v>0</v>
-      </c>
-      <c r="C11" s="15">
-        <f t="shared" si="0"/>
-        <v>-6.9077552789821368</v>
-      </c>
-      <c r="D11" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="16">
-        <v>0.35</v>
-      </c>
-      <c r="G11" s="15">
-        <v>90</v>
-      </c>
-      <c r="H11" s="15">
-        <v>90</v>
-      </c>
-      <c r="I11" s="15">
-        <v>90</v>
-      </c>
-      <c r="J11" s="15">
-        <v>100</v>
-      </c>
-      <c r="K11" s="15">
-        <v>80</v>
-      </c>
-      <c r="L11" s="31">
-        <f t="shared" si="2"/>
-        <v>86.666666666666671</v>
-      </c>
-      <c r="M11" s="20">
-        <v>5.6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="B12" s="15">
-        <v>0</v>
-      </c>
-      <c r="C12" s="15">
-        <f t="shared" si="0"/>
-        <v>-6.9077552789821368</v>
-      </c>
-      <c r="D12" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E12" s="15">
-        <v>0</v>
-      </c>
-      <c r="F12" s="16">
-        <v>0.38552361396303902</v>
-      </c>
-      <c r="G12" s="15">
-        <v>90</v>
-      </c>
-      <c r="H12" s="15">
-        <v>80</v>
-      </c>
-      <c r="I12" s="15">
-        <v>100</v>
-      </c>
-      <c r="J12" s="15">
-        <v>90</v>
-      </c>
-      <c r="K12" s="15">
-        <v>90</v>
-      </c>
-      <c r="L12" s="31">
-        <f t="shared" si="2"/>
-        <v>86.666666666666671</v>
-      </c>
-      <c r="M12" s="20">
-        <v>4.9000000000000004</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="B13" s="15">
-        <v>8</v>
-      </c>
-      <c r="C13" s="15">
-        <f t="shared" si="0"/>
-        <v>2.079566533867987</v>
-      </c>
-      <c r="D13" s="15">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="F13" s="16">
-        <v>0.47723201659281606</v>
-      </c>
-      <c r="G13" s="15">
-        <v>90</v>
-      </c>
-      <c r="H13" s="15">
-        <v>80</v>
-      </c>
-      <c r="I13" s="15">
-        <v>90</v>
-      </c>
-      <c r="J13" s="15">
-        <v>100</v>
-      </c>
-      <c r="K13" s="15">
-        <v>60</v>
-      </c>
-      <c r="L13" s="31">
-        <f t="shared" si="2"/>
-        <v>76.666666666666671</v>
-      </c>
-      <c r="M13" s="20">
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="B14" s="15">
-        <v>0</v>
-      </c>
-      <c r="C14" s="15">
-        <f t="shared" si="0"/>
-        <v>-6.9077552789821368</v>
-      </c>
-      <c r="D14" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E14" s="15">
-        <v>0</v>
-      </c>
-      <c r="F14" s="16">
-        <v>0.42186580341377283</v>
-      </c>
-      <c r="G14" s="15">
-        <v>100</v>
-      </c>
-      <c r="H14" s="15">
-        <v>100</v>
-      </c>
-      <c r="I14" s="15">
-        <v>100</v>
-      </c>
-      <c r="J14" s="15">
-        <v>100</v>
-      </c>
-      <c r="K14" s="15">
-        <v>90</v>
-      </c>
-      <c r="L14" s="31">
-        <f t="shared" si="2"/>
-        <v>96.666666666666671</v>
-      </c>
-      <c r="M14" s="20">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="B15" s="15">
-        <v>11</v>
-      </c>
-      <c r="C15" s="15">
-        <f t="shared" si="0"/>
-        <v>2.3979861777572986</v>
-      </c>
-      <c r="D15" s="15">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E15" s="15">
-        <v>0</v>
-      </c>
-      <c r="F15" s="16">
-        <v>0.43765652951699463</v>
-      </c>
-      <c r="G15" s="15">
-        <v>100</v>
-      </c>
-      <c r="H15" s="15">
-        <v>100</v>
-      </c>
-      <c r="I15" s="15">
-        <v>90</v>
-      </c>
-      <c r="J15" s="15">
-        <v>100</v>
-      </c>
-      <c r="K15" s="15">
-        <v>80</v>
-      </c>
-      <c r="L15" s="31">
-        <f t="shared" si="2"/>
-        <v>93.333333333333329</v>
-      </c>
-      <c r="M15" s="20">
-        <v>3.7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="B16" s="15">
-        <v>0</v>
-      </c>
-      <c r="C16" s="15">
-        <f t="shared" si="0"/>
-        <v>-6.9077552789821368</v>
-      </c>
-      <c r="D16" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="F16" s="16">
-        <v>0.35168693269395451</v>
-      </c>
-      <c r="G16" s="15">
-        <v>100</v>
-      </c>
-      <c r="H16" s="15">
-        <v>100</v>
-      </c>
-      <c r="I16" s="15">
-        <v>90</v>
-      </c>
-      <c r="J16" s="15">
-        <v>100</v>
-      </c>
-      <c r="K16" s="15">
-        <v>90</v>
-      </c>
-      <c r="L16" s="31">
-        <f t="shared" si="2"/>
-        <v>96.666666666666671</v>
-      </c>
-      <c r="M16" s="20">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13">
-      <c r="A17" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="B17" s="15">
-        <v>0</v>
-      </c>
-      <c r="C17" s="15">
-        <f t="shared" si="0"/>
-        <v>-6.9077552789821368</v>
-      </c>
-      <c r="D17" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="F17" s="16">
-        <v>0.39903746992093503</v>
-      </c>
-      <c r="G17" s="15">
-        <v>100</v>
-      </c>
-      <c r="H17" s="15">
-        <v>90</v>
-      </c>
-      <c r="I17" s="15">
-        <v>80</v>
-      </c>
-      <c r="J17" s="15">
-        <v>100</v>
-      </c>
-      <c r="K17" s="15">
-        <v>100</v>
-      </c>
-      <c r="L17" s="31">
-        <f t="shared" si="2"/>
-        <v>96.666666666666671</v>
-      </c>
-      <c r="M17" s="20">
-        <v>6.2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13">
-      <c r="A18" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="B18" s="15">
-        <v>12</v>
-      </c>
-      <c r="C18" s="15">
-        <f t="shared" si="0"/>
-        <v>2.4849899796493045</v>
-      </c>
-      <c r="D18" s="15">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E18" s="15">
-        <v>0</v>
-      </c>
-      <c r="F18" s="16">
-        <v>0.34517704517704506</v>
-      </c>
-      <c r="G18" s="15">
-        <v>80</v>
-      </c>
-      <c r="H18" s="15">
-        <v>100</v>
-      </c>
-      <c r="I18" s="15">
-        <v>100</v>
-      </c>
-      <c r="J18" s="15">
-        <v>100</v>
-      </c>
-      <c r="K18" s="15">
-        <v>100</v>
-      </c>
-      <c r="L18" s="31">
-        <f t="shared" si="2"/>
-        <v>93.333333333333329</v>
-      </c>
-      <c r="M18" s="20">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13">
-      <c r="A19" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="B19" s="15">
-        <v>0</v>
-      </c>
-      <c r="C19" s="15">
-        <f t="shared" si="0"/>
-        <v>-6.9077552789821368</v>
-      </c>
-      <c r="D19" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="F19" s="16">
-        <v>0.40032626427406193</v>
-      </c>
-      <c r="G19" s="15">
-        <v>90</v>
-      </c>
-      <c r="H19" s="15">
-        <v>20</v>
-      </c>
-      <c r="I19" s="15">
-        <v>100</v>
-      </c>
-      <c r="J19" s="15">
-        <v>100</v>
-      </c>
-      <c r="K19" s="15">
-        <v>40</v>
-      </c>
-      <c r="L19" s="31">
-        <f>AVERAGE(G19,H19,K19)</f>
-        <v>50</v>
-      </c>
-      <c r="M19" s="20">
-        <v>3.9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13">
-      <c r="A20" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="B20" s="15">
-        <v>0</v>
-      </c>
-      <c r="C20" s="15">
-        <f t="shared" si="0"/>
-        <v>-6.9077552789821368</v>
-      </c>
-      <c r="D20" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E20" s="15">
-        <v>0</v>
-      </c>
-      <c r="F20" s="16">
-        <v>0.37900023359028256</v>
-      </c>
-      <c r="G20" s="15">
-        <v>70</v>
-      </c>
-      <c r="H20" s="15">
-        <v>90</v>
-      </c>
-      <c r="I20" s="15">
-        <v>90</v>
-      </c>
-      <c r="J20" s="15">
-        <v>90</v>
-      </c>
-      <c r="K20" s="15">
-        <v>80</v>
-      </c>
-      <c r="L20" s="31">
-        <f t="shared" ref="L20:L35" si="3">AVERAGE(G20,H20,K20)</f>
-        <v>80</v>
-      </c>
-      <c r="M20" s="20">
-        <v>13.9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13">
-      <c r="A21" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="B21" s="15">
-        <v>28</v>
-      </c>
-      <c r="C21" s="15">
-        <f t="shared" si="0"/>
-        <v>3.3322402238231783</v>
-      </c>
-      <c r="D21" s="15">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="F21" s="16">
-        <v>0.41577181208053687</v>
-      </c>
-      <c r="G21" s="15">
-        <v>60</v>
-      </c>
-      <c r="H21" s="15">
-        <v>80</v>
-      </c>
-      <c r="I21" s="15">
-        <v>70</v>
-      </c>
-      <c r="J21" s="15">
-        <v>90</v>
-      </c>
-      <c r="K21" s="15">
-        <v>70</v>
-      </c>
-      <c r="L21" s="31">
-        <f t="shared" si="3"/>
-        <v>70</v>
-      </c>
-      <c r="M21" s="20">
-        <v>3.1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13">
-      <c r="A22" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="B22" s="15">
-        <v>15</v>
-      </c>
-      <c r="C22" s="15">
-        <f t="shared" si="0"/>
-        <v>2.7081168655467533</v>
-      </c>
-      <c r="D22" s="15">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="F22" s="16">
-        <v>0.45123674911660783</v>
-      </c>
-      <c r="G22" s="15">
-        <v>70</v>
-      </c>
-      <c r="H22" s="15">
-        <v>30</v>
-      </c>
-      <c r="I22" s="15">
-        <v>90</v>
-      </c>
-      <c r="J22" s="15">
-        <v>60</v>
-      </c>
-      <c r="K22" s="15">
-        <v>80</v>
-      </c>
-      <c r="L22" s="31">
-        <f t="shared" si="3"/>
-        <v>60</v>
-      </c>
-      <c r="M22" s="20">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13">
-      <c r="A23" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="B23" s="15">
-        <v>44</v>
-      </c>
-      <c r="C23" s="15">
-        <f t="shared" si="0"/>
-        <v>3.7842123609327278</v>
-      </c>
-      <c r="D23" s="15">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E23" s="15">
-        <v>0</v>
-      </c>
-      <c r="F23" s="16">
-        <v>0.31794248683677606</v>
-      </c>
-      <c r="G23" s="15">
-        <v>70</v>
-      </c>
-      <c r="H23" s="15">
-        <v>50</v>
-      </c>
-      <c r="I23" s="15">
-        <v>90</v>
-      </c>
-      <c r="J23" s="15">
-        <v>90</v>
-      </c>
-      <c r="K23" s="15">
-        <v>90</v>
-      </c>
-      <c r="L23" s="31">
-        <f t="shared" si="3"/>
-        <v>70</v>
-      </c>
-      <c r="M23" s="20">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13">
-      <c r="A24" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="B24" s="15">
-        <v>0</v>
-      </c>
-      <c r="C24" s="15">
-        <f t="shared" si="0"/>
-        <v>-6.9077552789821368</v>
-      </c>
-      <c r="D24" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="F24" s="16">
-        <v>0.43278185603155483</v>
-      </c>
-      <c r="G24" s="15">
-        <v>70</v>
-      </c>
-      <c r="H24" s="15">
-        <v>90</v>
-      </c>
-      <c r="I24" s="15">
-        <v>90</v>
-      </c>
-      <c r="J24" s="15">
-        <v>100</v>
-      </c>
-      <c r="K24" s="15">
-        <v>40</v>
-      </c>
-      <c r="L24" s="31">
-        <f t="shared" si="3"/>
-        <v>66.666666666666671</v>
-      </c>
-      <c r="M24" s="20">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13">
-      <c r="A25" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="B25" s="15">
-        <v>0</v>
-      </c>
-      <c r="C25" s="15">
-        <f t="shared" si="0"/>
-        <v>-6.9077552789821368</v>
-      </c>
-      <c r="D25" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="F25" s="16">
-        <v>0.40381439894319682</v>
-      </c>
-      <c r="G25" s="15">
-        <v>40</v>
-      </c>
-      <c r="H25" s="15">
-        <v>60</v>
-      </c>
-      <c r="I25" s="15">
-        <v>100</v>
-      </c>
-      <c r="J25" s="15">
-        <v>100</v>
-      </c>
-      <c r="K25" s="15">
-        <v>80</v>
-      </c>
-      <c r="L25" s="31">
-        <f t="shared" si="3"/>
-        <v>60</v>
-      </c>
-      <c r="M25" s="20">
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13">
-      <c r="A26" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="B26" s="15">
-        <v>0</v>
-      </c>
-      <c r="C26" s="15">
-        <f t="shared" si="0"/>
-        <v>-6.9077552789821368</v>
-      </c>
-      <c r="D26" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="F26" s="16">
-        <v>0.23604106628242064</v>
-      </c>
-      <c r="G26" s="15">
-        <v>80</v>
-      </c>
-      <c r="H26" s="15">
-        <v>90</v>
-      </c>
-      <c r="I26" s="15">
-        <v>90</v>
-      </c>
-      <c r="J26" s="15">
-        <v>90</v>
-      </c>
-      <c r="K26" s="15">
-        <v>40</v>
-      </c>
-      <c r="L26" s="31">
-        <f t="shared" si="3"/>
-        <v>70</v>
-      </c>
-      <c r="M26" s="20">
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13">
-      <c r="A27" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="B27" s="15">
-        <v>12</v>
-      </c>
-      <c r="C27" s="15">
-        <f t="shared" si="0"/>
-        <v>2.4849899796493045</v>
-      </c>
-      <c r="D27" s="15">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E27" s="15">
-        <v>0</v>
-      </c>
-      <c r="F27" s="16">
-        <v>0.39749423013517965</v>
-      </c>
-      <c r="G27" s="15">
-        <v>70</v>
-      </c>
-      <c r="H27" s="15">
-        <v>90</v>
-      </c>
-      <c r="I27" s="15">
-        <v>100</v>
-      </c>
-      <c r="J27" s="15">
-        <v>90</v>
-      </c>
-      <c r="K27" s="15">
-        <v>80</v>
-      </c>
-      <c r="L27" s="31">
-        <f t="shared" si="3"/>
-        <v>80</v>
-      </c>
-      <c r="M27" s="20">
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13">
-      <c r="A28" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="B28" s="15">
-        <v>0</v>
-      </c>
-      <c r="C28" s="15">
-        <f t="shared" si="0"/>
-        <v>-6.9077552789821368</v>
-      </c>
-      <c r="D28" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E28" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="F28" s="16">
-        <v>0.44650666666666666</v>
-      </c>
-      <c r="G28" s="15">
-        <v>90</v>
-      </c>
-      <c r="H28" s="15">
-        <v>90</v>
-      </c>
-      <c r="I28" s="15">
-        <v>90</v>
-      </c>
-      <c r="J28" s="15">
-        <v>100</v>
-      </c>
-      <c r="K28" s="15">
-        <v>80</v>
-      </c>
-      <c r="L28" s="31">
-        <f t="shared" si="3"/>
-        <v>86.666666666666671</v>
-      </c>
-      <c r="M28" s="20">
-        <v>5.6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13">
-      <c r="A29" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="B29" s="15">
-        <v>0</v>
-      </c>
-      <c r="C29" s="15">
-        <f t="shared" si="0"/>
-        <v>-6.9077552789821368</v>
-      </c>
-      <c r="D29" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E29" s="15">
-        <v>0</v>
-      </c>
-      <c r="F29" s="16">
-        <v>0.43278185603155483</v>
-      </c>
-      <c r="G29" s="15">
-        <v>90</v>
-      </c>
-      <c r="H29" s="15">
-        <v>80</v>
-      </c>
-      <c r="I29" s="15">
-        <v>100</v>
-      </c>
-      <c r="J29" s="15">
-        <v>90</v>
-      </c>
-      <c r="K29" s="15">
-        <v>90</v>
-      </c>
-      <c r="L29" s="31">
-        <f t="shared" si="3"/>
-        <v>86.666666666666671</v>
-      </c>
-      <c r="M29" s="20">
-        <v>4.9000000000000004</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13">
-      <c r="A30" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="B30" s="15">
-        <v>13</v>
-      </c>
-      <c r="C30" s="15">
-        <f t="shared" si="0"/>
-        <v>2.5650262775800314</v>
-      </c>
-      <c r="D30" s="15">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="F30" s="16">
-        <v>0.40480961923847691</v>
-      </c>
-      <c r="G30" s="15">
-        <v>90</v>
-      </c>
-      <c r="H30" s="15">
-        <v>80</v>
-      </c>
-      <c r="I30" s="15">
-        <v>90</v>
-      </c>
-      <c r="J30" s="15">
-        <v>100</v>
-      </c>
-      <c r="K30" s="15">
-        <v>60</v>
-      </c>
-      <c r="L30" s="31">
-        <f t="shared" si="3"/>
-        <v>76.666666666666671</v>
-      </c>
-      <c r="M30" s="20">
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13">
-      <c r="A31" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="B31" s="15">
-        <v>0</v>
-      </c>
-      <c r="C31" s="15">
-        <f t="shared" si="0"/>
-        <v>-6.9077552789821368</v>
-      </c>
-      <c r="D31" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E31" s="15">
-        <v>0</v>
-      </c>
-      <c r="F31" s="16">
-        <v>0.415685987866384</v>
-      </c>
-      <c r="G31" s="15">
-        <v>100</v>
-      </c>
-      <c r="H31" s="15">
-        <v>100</v>
-      </c>
-      <c r="I31" s="15">
-        <v>100</v>
-      </c>
-      <c r="J31" s="15">
-        <v>100</v>
-      </c>
-      <c r="K31" s="15">
-        <v>90</v>
-      </c>
-      <c r="L31" s="31">
-        <f t="shared" si="3"/>
-        <v>96.666666666666671</v>
-      </c>
-      <c r="M31" s="20">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13">
-      <c r="A32" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="B32" s="15">
-        <v>14</v>
-      </c>
-      <c r="C32" s="15">
-        <f t="shared" si="0"/>
-        <v>2.6391287556357881</v>
-      </c>
-      <c r="D32" s="15">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E32" s="15">
-        <v>0</v>
-      </c>
-      <c r="F32" s="16">
-        <v>0.41123247473100755</v>
-      </c>
-      <c r="G32" s="15">
-        <v>100</v>
-      </c>
-      <c r="H32" s="15">
-        <v>100</v>
-      </c>
-      <c r="I32" s="15">
-        <v>90</v>
-      </c>
-      <c r="J32" s="15">
-        <v>100</v>
-      </c>
-      <c r="K32" s="15">
-        <v>80</v>
-      </c>
-      <c r="L32" s="31">
-        <f t="shared" si="3"/>
-        <v>93.333333333333329</v>
-      </c>
-      <c r="M32" s="20">
-        <v>3.7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13">
-      <c r="A33" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="B33" s="15">
-        <v>0</v>
-      </c>
-      <c r="C33" s="15">
-        <f t="shared" si="0"/>
-        <v>-6.9077552789821368</v>
-      </c>
-      <c r="D33" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E33" s="15">
-        <v>0</v>
-      </c>
-      <c r="F33" s="16">
-        <v>0.30132343447385412</v>
-      </c>
-      <c r="G33" s="15">
-        <v>100</v>
-      </c>
-      <c r="H33" s="15">
-        <v>100</v>
-      </c>
-      <c r="I33" s="15">
-        <v>90</v>
-      </c>
-      <c r="J33" s="15">
-        <v>100</v>
-      </c>
-      <c r="K33" s="15">
-        <v>90</v>
-      </c>
-      <c r="L33" s="31">
-        <f t="shared" si="3"/>
-        <v>96.666666666666671</v>
-      </c>
-      <c r="M33" s="20">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13">
-      <c r="A34" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="B34" s="15">
-        <v>0</v>
-      </c>
-      <c r="C34" s="15">
-        <f t="shared" si="0"/>
-        <v>-6.9077552789821368</v>
-      </c>
-      <c r="D34" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E34" s="15">
-        <v>0</v>
-      </c>
-      <c r="F34" s="16">
-        <v>0.3078115313081215</v>
-      </c>
-      <c r="G34" s="15">
-        <v>100</v>
-      </c>
-      <c r="H34" s="15">
-        <v>90</v>
-      </c>
-      <c r="I34" s="15">
-        <v>80</v>
-      </c>
-      <c r="J34" s="15">
-        <v>100</v>
-      </c>
-      <c r="K34" s="15">
-        <v>100</v>
-      </c>
-      <c r="L34" s="31">
-        <f t="shared" si="3"/>
-        <v>96.666666666666671</v>
-      </c>
-      <c r="M34" s="20">
-        <v>6.2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13">
-      <c r="A35" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="B35" s="15">
-        <v>15</v>
-      </c>
-      <c r="C35" s="15">
-        <f t="shared" si="0"/>
-        <v>2.7081168655467533</v>
-      </c>
-      <c r="D35" s="15">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E35" s="15">
-        <v>0</v>
-      </c>
-      <c r="F35" s="16">
-        <v>0.35321692253603648</v>
-      </c>
-      <c r="G35" s="15">
-        <v>80</v>
-      </c>
-      <c r="H35" s="15">
-        <v>100</v>
-      </c>
-      <c r="I35" s="15">
-        <v>100</v>
-      </c>
-      <c r="J35" s="15">
-        <v>100</v>
-      </c>
-      <c r="K35" s="15">
-        <v>100</v>
-      </c>
-      <c r="L35" s="31">
-        <f t="shared" si="3"/>
-        <v>93.333333333333329</v>
-      </c>
-      <c r="M35" s="20">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13">
-      <c r="A36" s="15">
-        <f>0.5+A19</f>
-        <v>0.75</v>
-      </c>
-      <c r="B36" s="15">
-        <v>0</v>
-      </c>
-      <c r="C36" s="15">
-        <f t="shared" si="0"/>
-        <v>-6.9077552789821368</v>
-      </c>
-      <c r="D36" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E36" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="F36" s="16">
-        <v>0.25809840658378569</v>
-      </c>
-      <c r="G36" s="15">
-        <v>90</v>
-      </c>
-      <c r="H36" s="15">
-        <v>20</v>
-      </c>
-      <c r="I36" s="15">
-        <v>100</v>
-      </c>
-      <c r="J36" s="15">
-        <v>100</v>
-      </c>
-      <c r="K36" s="15">
-        <v>40</v>
-      </c>
-      <c r="L36" s="31">
-        <f>AVERAGE(G36,H36,K36)</f>
-        <v>50</v>
-      </c>
-      <c r="M36" s="15">
-        <v>3.9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13">
-      <c r="A37" s="15">
-        <f t="shared" ref="A37:A52" si="4">0.5+A20</f>
-        <v>0.75</v>
-      </c>
-      <c r="B37" s="15">
-        <v>0</v>
-      </c>
-      <c r="C37" s="15">
-        <f t="shared" si="0"/>
-        <v>-6.9077552789821368</v>
-      </c>
-      <c r="D37" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E37" s="15">
-        <v>0</v>
-      </c>
-      <c r="F37" s="16">
-        <v>0.11742526259089683</v>
-      </c>
-      <c r="G37" s="15">
-        <v>70</v>
-      </c>
-      <c r="H37" s="15">
-        <v>90</v>
-      </c>
-      <c r="I37" s="15">
-        <v>90</v>
-      </c>
-      <c r="J37" s="15">
-        <v>90</v>
-      </c>
-      <c r="K37" s="15">
-        <v>80</v>
-      </c>
-      <c r="L37" s="31">
-        <f t="shared" ref="L37:L52" si="5">AVERAGE(G37,H37,K37)</f>
-        <v>80</v>
-      </c>
-      <c r="M37" s="15">
-        <v>13.9</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13">
-      <c r="A38" s="15">
-        <f t="shared" si="4"/>
-        <v>0.75</v>
-      </c>
-      <c r="B38" s="15">
-        <v>0</v>
-      </c>
-      <c r="C38" s="15">
-        <f t="shared" si="0"/>
-        <v>-6.9077552789821368</v>
-      </c>
-      <c r="D38" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E38" s="15">
-        <v>0</v>
-      </c>
-      <c r="F38" s="16">
-        <v>0.23132451055452269</v>
-      </c>
-      <c r="G38" s="15">
-        <v>60</v>
-      </c>
-      <c r="H38" s="15">
-        <v>80</v>
-      </c>
-      <c r="I38" s="15">
-        <v>70</v>
-      </c>
-      <c r="J38" s="15">
-        <v>90</v>
-      </c>
-      <c r="K38" s="15">
-        <v>70</v>
-      </c>
-      <c r="L38" s="31">
-        <f t="shared" si="5"/>
-        <v>70</v>
-      </c>
-      <c r="M38" s="15">
-        <v>3.1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13">
-      <c r="A39" s="15">
-        <f t="shared" si="4"/>
-        <v>0.75</v>
-      </c>
-      <c r="B39" s="15">
-        <v>1</v>
-      </c>
-      <c r="C39" s="15">
-        <f t="shared" si="0"/>
-        <v>9.9950033308342321E-4</v>
-      </c>
-      <c r="D39" s="15">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E39" s="15">
-        <v>0</v>
-      </c>
-      <c r="F39" s="16">
-        <v>0.38323477539163808</v>
-      </c>
-      <c r="G39" s="15">
-        <v>70</v>
-      </c>
-      <c r="H39" s="15">
-        <v>30</v>
-      </c>
-      <c r="I39" s="15">
-        <v>90</v>
-      </c>
-      <c r="J39" s="15">
-        <v>60</v>
-      </c>
-      <c r="K39" s="15">
-        <v>80</v>
-      </c>
-      <c r="L39" s="31">
-        <f t="shared" si="5"/>
-        <v>60</v>
-      </c>
-      <c r="M39" s="20">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13">
-      <c r="A40" s="15">
-        <f t="shared" si="4"/>
-        <v>0.75</v>
-      </c>
-      <c r="B40" s="15">
-        <v>0</v>
-      </c>
-      <c r="C40" s="15">
-        <f t="shared" si="0"/>
-        <v>-6.9077552789821368</v>
-      </c>
-      <c r="D40" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E40" s="15">
-        <v>0</v>
-      </c>
-      <c r="F40" s="16">
-        <v>0.29475043029259906</v>
-      </c>
-      <c r="G40" s="15">
-        <v>70</v>
-      </c>
-      <c r="H40" s="15">
-        <v>50</v>
-      </c>
-      <c r="I40" s="15">
-        <v>90</v>
-      </c>
-      <c r="J40" s="15">
-        <v>90</v>
-      </c>
-      <c r="K40" s="15">
-        <v>90</v>
-      </c>
-      <c r="L40" s="31">
-        <f t="shared" si="5"/>
-        <v>70</v>
-      </c>
-      <c r="M40" s="20">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13">
-      <c r="A41" s="15">
-        <f t="shared" si="4"/>
-        <v>0.75</v>
-      </c>
-      <c r="B41" s="15">
-        <v>0</v>
-      </c>
-      <c r="C41" s="15">
-        <f t="shared" si="0"/>
-        <v>-6.9077552789821368</v>
-      </c>
-      <c r="D41" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E41" s="15">
-        <v>0</v>
-      </c>
-      <c r="F41" s="16">
-        <v>0.26349390597794553</v>
-      </c>
-      <c r="G41" s="15">
-        <v>70</v>
-      </c>
-      <c r="H41" s="15">
-        <v>90</v>
-      </c>
-      <c r="I41" s="15">
-        <v>90</v>
-      </c>
-      <c r="J41" s="15">
-        <v>100</v>
-      </c>
-      <c r="K41" s="15">
-        <v>40</v>
-      </c>
-      <c r="L41" s="31">
-        <f t="shared" si="5"/>
-        <v>66.666666666666671</v>
-      </c>
-      <c r="M41" s="20">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13">
-      <c r="A42" s="15">
-        <f t="shared" si="4"/>
-        <v>0.75</v>
-      </c>
-      <c r="B42" s="15">
-        <v>0</v>
-      </c>
-      <c r="C42" s="15">
-        <f t="shared" si="0"/>
-        <v>-6.9077552789821368</v>
-      </c>
-      <c r="D42" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E42" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="F42" s="16">
-        <v>0.27677564825253659</v>
-      </c>
-      <c r="G42" s="15">
-        <v>40</v>
-      </c>
-      <c r="H42" s="15">
-        <v>60</v>
-      </c>
-      <c r="I42" s="15">
-        <v>100</v>
-      </c>
-      <c r="J42" s="15">
-        <v>100</v>
-      </c>
-      <c r="K42" s="15">
-        <v>80</v>
-      </c>
-      <c r="L42" s="31">
-        <f t="shared" si="5"/>
-        <v>60</v>
-      </c>
-      <c r="M42" s="20">
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13">
-      <c r="A43" s="15">
-        <f t="shared" si="4"/>
-        <v>0.75</v>
-      </c>
-      <c r="B43" s="15">
-        <v>0</v>
-      </c>
-      <c r="C43" s="15">
-        <f t="shared" si="0"/>
-        <v>-6.9077552789821368</v>
-      </c>
-      <c r="D43" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E43" s="15">
-        <v>0</v>
-      </c>
-      <c r="F43" s="16">
-        <v>0.27963737796373783</v>
-      </c>
-      <c r="G43" s="15">
-        <v>80</v>
-      </c>
-      <c r="H43" s="15">
-        <v>90</v>
-      </c>
-      <c r="I43" s="15">
-        <v>90</v>
-      </c>
-      <c r="J43" s="15">
-        <v>90</v>
-      </c>
-      <c r="K43" s="15">
-        <v>40</v>
-      </c>
-      <c r="L43" s="31">
-        <f t="shared" si="5"/>
-        <v>70</v>
-      </c>
-      <c r="M43" s="20">
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13">
-      <c r="A44" s="15">
-        <f t="shared" si="4"/>
-        <v>0.75</v>
-      </c>
-      <c r="B44" s="15">
-        <v>0</v>
-      </c>
-      <c r="C44" s="15">
-        <f t="shared" si="0"/>
-        <v>-6.9077552789821368</v>
-      </c>
-      <c r="D44" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E44" s="15">
-        <v>0</v>
-      </c>
-      <c r="F44" s="16">
-        <v>0.29137630662020902</v>
-      </c>
-      <c r="G44" s="15">
-        <v>70</v>
-      </c>
-      <c r="H44" s="15">
-        <v>90</v>
-      </c>
-      <c r="I44" s="15">
-        <v>100</v>
-      </c>
-      <c r="J44" s="15">
-        <v>90</v>
-      </c>
-      <c r="K44" s="15">
-        <v>80</v>
-      </c>
-      <c r="L44" s="31">
-        <f t="shared" si="5"/>
-        <v>80</v>
-      </c>
-      <c r="M44" s="20">
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13">
-      <c r="A45" s="15">
-        <f t="shared" si="4"/>
-        <v>0.75</v>
-      </c>
-      <c r="B45" s="15">
-        <v>0</v>
-      </c>
-      <c r="C45" s="15">
-        <f t="shared" si="0"/>
-        <v>-6.9077552789821368</v>
-      </c>
-      <c r="D45" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E45" s="15">
-        <v>0</v>
-      </c>
-      <c r="F45" s="16">
-        <v>0.40324158166829677</v>
-      </c>
-      <c r="G45" s="15">
-        <v>90</v>
-      </c>
-      <c r="H45" s="15">
-        <v>90</v>
-      </c>
-      <c r="I45" s="15">
-        <v>90</v>
-      </c>
-      <c r="J45" s="15">
-        <v>100</v>
-      </c>
-      <c r="K45" s="15">
-        <v>80</v>
-      </c>
-      <c r="L45" s="31">
-        <f t="shared" si="5"/>
-        <v>86.666666666666671</v>
-      </c>
-      <c r="M45" s="20">
-        <v>5.6</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13">
-      <c r="A46" s="15">
-        <f t="shared" si="4"/>
-        <v>0.75</v>
-      </c>
-      <c r="B46" s="15">
-        <v>0</v>
-      </c>
-      <c r="C46" s="15">
-        <f t="shared" si="0"/>
-        <v>-6.9077552789821368</v>
-      </c>
-      <c r="D46" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E46" s="15">
-        <v>0</v>
-      </c>
-      <c r="F46" s="16">
-        <v>0.38038679840235445</v>
-      </c>
-      <c r="G46" s="15">
-        <v>90</v>
-      </c>
-      <c r="H46" s="15">
-        <v>80</v>
-      </c>
-      <c r="I46" s="15">
-        <v>100</v>
-      </c>
-      <c r="J46" s="15">
-        <v>90</v>
-      </c>
-      <c r="K46" s="15">
-        <v>90</v>
-      </c>
-      <c r="L46" s="31">
-        <f t="shared" si="5"/>
-        <v>86.666666666666671</v>
-      </c>
-      <c r="M46" s="20">
-        <v>4.9000000000000004</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13">
-      <c r="A47" s="15">
-        <f t="shared" si="4"/>
-        <v>0.75</v>
-      </c>
-      <c r="B47" s="15">
-        <v>0</v>
-      </c>
-      <c r="C47" s="15">
-        <f t="shared" si="0"/>
-        <v>-6.9077552789821368</v>
-      </c>
-      <c r="D47" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E47" s="15">
-        <v>0</v>
-      </c>
-      <c r="F47" s="16">
-        <v>0.24292995725090433</v>
-      </c>
-      <c r="G47" s="15">
-        <v>90</v>
-      </c>
-      <c r="H47" s="15">
-        <v>80</v>
-      </c>
-      <c r="I47" s="15">
-        <v>90</v>
-      </c>
-      <c r="J47" s="15">
-        <v>100</v>
-      </c>
-      <c r="K47" s="15">
-        <v>60</v>
-      </c>
-      <c r="L47" s="31">
-        <f t="shared" si="5"/>
-        <v>76.666666666666671</v>
-      </c>
-      <c r="M47" s="20">
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13">
-      <c r="A48" s="15">
-        <f t="shared" si="4"/>
-        <v>0.75</v>
-      </c>
-      <c r="B48" s="15">
-        <v>0</v>
-      </c>
-      <c r="C48" s="15">
-        <f t="shared" si="0"/>
-        <v>-6.9077552789821368</v>
-      </c>
-      <c r="D48" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E48" s="15">
-        <v>0</v>
-      </c>
-      <c r="F48" s="16">
-        <v>0.169047619047619</v>
-      </c>
-      <c r="G48" s="15">
-        <v>100</v>
-      </c>
-      <c r="H48" s="15">
-        <v>100</v>
-      </c>
-      <c r="I48" s="15">
-        <v>100</v>
-      </c>
-      <c r="J48" s="15">
-        <v>100</v>
-      </c>
-      <c r="K48" s="15">
-        <v>90</v>
-      </c>
-      <c r="L48" s="31">
-        <f t="shared" si="5"/>
-        <v>96.666666666666671</v>
-      </c>
-      <c r="M48" s="20">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13">
-      <c r="A49" s="15">
-        <f t="shared" si="4"/>
-        <v>0.75</v>
-      </c>
-      <c r="B49" s="15">
-        <v>1</v>
-      </c>
-      <c r="C49" s="15">
-        <f t="shared" si="0"/>
-        <v>9.9950033308342321E-4</v>
-      </c>
-      <c r="D49" s="15">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E49" s="15">
-        <v>0</v>
-      </c>
-      <c r="F49" s="16">
-        <v>0.27698226116691604</v>
-      </c>
-      <c r="G49" s="15">
-        <v>100</v>
-      </c>
-      <c r="H49" s="15">
-        <v>100</v>
-      </c>
-      <c r="I49" s="15">
-        <v>90</v>
-      </c>
-      <c r="J49" s="15">
-        <v>100</v>
-      </c>
-      <c r="K49" s="15">
-        <v>80</v>
-      </c>
-      <c r="L49" s="31">
-        <f t="shared" si="5"/>
-        <v>93.333333333333329</v>
-      </c>
-      <c r="M49" s="20">
-        <v>3.7</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13">
-      <c r="A50" s="15">
-        <f t="shared" si="4"/>
-        <v>0.75</v>
-      </c>
-      <c r="B50" s="15">
-        <v>0</v>
-      </c>
-      <c r="C50" s="15">
-        <f t="shared" si="0"/>
-        <v>-6.9077552789821368</v>
-      </c>
-      <c r="D50" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E50" s="15">
-        <v>0</v>
-      </c>
-      <c r="F50" s="16">
-        <v>0.25380258899676367</v>
-      </c>
-      <c r="G50" s="15">
-        <v>100</v>
-      </c>
-      <c r="H50" s="15">
-        <v>100</v>
-      </c>
-      <c r="I50" s="15">
-        <v>90</v>
-      </c>
-      <c r="J50" s="15">
-        <v>100</v>
-      </c>
-      <c r="K50" s="15">
-        <v>90</v>
-      </c>
-      <c r="L50" s="31">
-        <f t="shared" si="5"/>
-        <v>96.666666666666671</v>
-      </c>
-      <c r="M50" s="20">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13">
-      <c r="A51" s="15">
-        <f t="shared" si="4"/>
-        <v>0.75</v>
-      </c>
-      <c r="B51" s="15">
-        <v>0</v>
-      </c>
-      <c r="C51" s="15">
-        <f t="shared" si="0"/>
-        <v>-6.9077552789821368</v>
-      </c>
-      <c r="D51" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E51" s="15">
-        <v>0</v>
-      </c>
-      <c r="F51" s="16">
-        <v>0.12557523357969599</v>
-      </c>
-      <c r="G51" s="15">
-        <v>100</v>
-      </c>
-      <c r="H51" s="15">
-        <v>90</v>
-      </c>
-      <c r="I51" s="15">
-        <v>80</v>
-      </c>
-      <c r="J51" s="15">
-        <v>100</v>
-      </c>
-      <c r="K51" s="15">
-        <v>100</v>
-      </c>
-      <c r="L51" s="31">
-        <f t="shared" si="5"/>
-        <v>96.666666666666671</v>
-      </c>
-      <c r="M51" s="20">
-        <v>6.2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13">
-      <c r="A52" s="15">
-        <f t="shared" si="4"/>
-        <v>0.75</v>
-      </c>
-      <c r="B52" s="15">
-        <v>0</v>
-      </c>
-      <c r="C52" s="15">
-        <f t="shared" si="0"/>
-        <v>-6.9077552789821368</v>
-      </c>
-      <c r="D52" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E52" s="15">
-        <v>0</v>
-      </c>
-      <c r="F52" s="16">
-        <v>0.39540306462358427</v>
-      </c>
-      <c r="G52" s="15">
-        <v>80</v>
-      </c>
-      <c r="H52" s="15">
-        <v>100</v>
-      </c>
-      <c r="I52" s="15">
-        <v>100</v>
-      </c>
-      <c r="J52" s="15">
-        <v>100</v>
-      </c>
-      <c r="K52" s="15">
-        <v>100</v>
-      </c>
-      <c r="L52" s="31">
-        <f t="shared" si="5"/>
-        <v>93.333333333333329</v>
-      </c>
-      <c r="M52" s="20">
-        <v>1.4</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>

</xml_diff>